<commit_message>
CHANGES IN THE CORRELATION TABLE TO SHOW BOTH INPUT & OUTPUT TOGETHER
</commit_message>
<xml_diff>
--- a/Documentation/Results and Analysis of Experiments/Local Area Density and Potential Radious.xlsx
+++ b/Documentation/Results and Analysis of Experiments/Local Area Density and Potential Radious.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarla\Desktop\PotentialRadious40\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRA-UAS\SoEng\git\Project\ImageClassification\NeoCortexApi-ImageClassificationMYWork\neocortexapi-classification\Documentation\Results and Analysis of Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0972DB-23C3-4093-8310-DF6C1EFF8F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95806F3-AA79-47F1-B085-D845F3DEA9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,7 +235,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Similarity between Hexagon1 &amp; Hexagon 2</a:t>
+              <a:t>Similarity between Hexagon1 &amp; Hexagon 2 </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(Local Inhibition)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1127,13 +1136,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1141,9 +1164,47 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1400"/>
               <a:t>Similarity between Hexagon1 &amp; Triangle 1</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(Local Inhibition)</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1159,13 +1220,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3949,8 +4024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>